<commit_message>
added variable description from the data dictionary for CAPER business
</commit_message>
<xml_diff>
--- a/var-master.xlsx
+++ b/var-master.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="9960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="army_master" sheetId="1" r:id="rId1"/>
+    <sheet name="caper_business" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="120">
   <si>
     <t>PID_PDE</t>
   </si>
@@ -213,13 +214,209 @@
   </si>
   <si>
     <t>No data dictionary available for this variable.</t>
+  </si>
+  <si>
+    <t>pid_pde_patient</t>
+  </si>
+  <si>
+    <t>unique patient id</t>
+  </si>
+  <si>
+    <t>pid_pde_sponsor</t>
+  </si>
+  <si>
+    <t>half the # of unique values as patient id</t>
+  </si>
+  <si>
+    <t>encounter_key</t>
+  </si>
+  <si>
+    <t>unique id for patient visit</t>
+  </si>
+  <si>
+    <t>each obs has a different id</t>
+  </si>
+  <si>
+    <t>assgndur</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>cptuos_1 - cptuos_3</t>
+  </si>
+  <si>
+    <t>mostly takes value 1</t>
+  </si>
+  <si>
+    <t>cptuos_4 - cptuos_13</t>
+  </si>
+  <si>
+    <t>mostly takes value 1, largely missing</t>
+  </si>
+  <si>
+    <t>msma</t>
+  </si>
+  <si>
+    <t>largely missing</t>
+  </si>
+  <si>
+    <t>npervu1</t>
+  </si>
+  <si>
+    <t>mostly takes val 0 or 1</t>
+  </si>
+  <si>
+    <t>npervu2 - npervu13</t>
+  </si>
+  <si>
+    <t>ntrvu</t>
+  </si>
+  <si>
+    <t>ntrvu1-ntrvu13</t>
+  </si>
+  <si>
+    <t>connected to npervu1-13?</t>
+  </si>
+  <si>
+    <t>nwrvu</t>
+  </si>
+  <si>
+    <t>never missing</t>
+  </si>
+  <si>
+    <t>nwrvu1-nwrvu13</t>
+  </si>
+  <si>
+    <t>p1pervu</t>
+  </si>
+  <si>
+    <t>p1pervu1 - p1pervu13</t>
+  </si>
+  <si>
+    <t>p1trvu</t>
+  </si>
+  <si>
+    <t>connected to p1pervu?</t>
+  </si>
+  <si>
+    <t>p1trvu1 - p1trvu13</t>
+  </si>
+  <si>
+    <t>p1wrvu</t>
+  </si>
+  <si>
+    <t>p1wrvu1 - p1wrvu13</t>
+  </si>
+  <si>
+    <t>rrvu1 - rrvu13</t>
+  </si>
+  <si>
+    <t>rvu_epe</t>
+  </si>
+  <si>
+    <t>rvu_et</t>
+  </si>
+  <si>
+    <t>skill1</t>
+  </si>
+  <si>
+    <t>Sponsor's ID - Not useful for military</t>
+  </si>
+  <si>
+    <t>How long the visit is scheduled to last</t>
+  </si>
+  <si>
+    <t>CPT units of service - quantity of each CPT</t>
+  </si>
+  <si>
+    <t>Same as above. 1-3 are E&amp;M, 4-13 are procedure codes</t>
+  </si>
+  <si>
+    <t>Regional identifier for certain areas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> non-provider affected  Practice Expense RVUs for each CPT after multiple procedure discounting, UOS and modifier impacts applied.</t>
+  </si>
+  <si>
+    <t>Sum of non-provider affected Work and Practice Expense RVUs for each CPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of non-provider affected  Work RVUs for all CPT after multiple procedure discounting, UOS and modifier impacts applied.  </t>
+  </si>
+  <si>
+    <t>Sum of non-provider affected Work and Practice Expense RVUs</t>
+  </si>
+  <si>
+    <t>Non-provider affected  Work RVUs for each CPT after multiple procedure discounting, UOS and modifier impacts applied.</t>
+  </si>
+  <si>
+    <t>Sum of Provider-affected Practice Expense RVUs  associated with each Provider.</t>
+  </si>
+  <si>
+    <t>Provider-affected Practice Expense RVUs associated with Provider K for each CPT.</t>
+  </si>
+  <si>
+    <t>Sum of Provider-affected Total RVUs  associated with each Provider.</t>
+  </si>
+  <si>
+    <t>Provider-affected Total RVUs associated with Provider K for each CPT.</t>
+  </si>
+  <si>
+    <t>Sum of Provider-affected Work RVUs  associated with each Provider.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sum of all Provider-affected Practice Expense RVUs for each CPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw MHS updated Work RVU of CPT J, derived from merge with CPT Weight Table and subject to modification </t>
+  </si>
+  <si>
+    <t>Sum of Practice Expense RVU, with modifiers, chosen based on designation as facility or non-facility care, multiplied by the units of service, computed as:
+∑(PERVUJ*CPTUOS_J) for all J CPT Codes</t>
+  </si>
+  <si>
+    <t>EPE stands for "Enhanced Practice Expense"</t>
+  </si>
+  <si>
+    <t>Total RVU's based on all 13 CPT</t>
+  </si>
+  <si>
+    <t>Skill Type based on CHCS Provider Specialty code.  This Skill Type is used when determining Provider RVUs.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="MS Reference Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="MS Reference Sans Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t>=1 to 5 represents Appointment Provider and Additional Providers 1 to 4.
+1,2 - Clinicians, Direct Care Professionals - considered privileged providers and eligible for multiple provider RVU credit.
+1R - Interns/Residents with license - eligible for RVU credit (except multiple provider RVU credit)
+3,4 - Nurses, Techs, Direct Care Para-Professionals, Residents without License - RVU credit only applicable on certain procedures.
+5 - Admin/Clerical - not eligible for RVU credit.
+G - Generic
+N - Inactive
+Populated for FY07+ only.
+No data are currently available for Additional Providers 3 and 4 (SKILL4 and SKILL5 are empty).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +432,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Reference Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="MS Reference Sans Serif"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -244,7 +457,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -252,19 +465,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 13" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -578,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -919,4 +1152,351 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="69.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="308" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added table of contents tab describing the data tables
</commit_message>
<xml_diff>
--- a/var-master.xlsx
+++ b/var-master.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="9960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="9960"/>
   </bookViews>
   <sheets>
-    <sheet name="army_master" sheetId="1" r:id="rId1"/>
-    <sheet name="caper_business" sheetId="2" r:id="rId2"/>
+    <sheet name="Table of Contents" sheetId="3" r:id="rId1"/>
+    <sheet name="army_master" sheetId="1" r:id="rId2"/>
+    <sheet name="caper_business" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="157">
   <si>
     <t>PID_PDE</t>
   </si>
@@ -410,6 +411,117 @@
 Populated for FY07+ only.
 No data are currently available for Additional Providers 3 and 4 (SKILL4 and SKILL5 are empty).</t>
     </r>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>army_master</t>
+  </si>
+  <si>
+    <t>caper_business</t>
+  </si>
+  <si>
+    <t>caper_patient</t>
+  </si>
+  <si>
+    <t>sidr_patient</t>
+  </si>
+  <si>
+    <t>sidr_provider</t>
+  </si>
+  <si>
+    <t>ted-I</t>
+  </si>
+  <si>
+    <t>TED-NI</t>
+  </si>
+  <si>
+    <t>PDTS</t>
+  </si>
+  <si>
+    <t>Unit of Analysis</t>
+  </si>
+  <si>
+    <t>individual servicemember</t>
+  </si>
+  <si>
+    <t>PID_NPI</t>
+  </si>
+  <si>
+    <t>crosswalk between military ID and NPI for anyone (military or civilian) with a patient encouner since third quarter 2012</t>
+  </si>
+  <si>
+    <t>Individual  Provider</t>
+  </si>
+  <si>
+    <t>PID_PDE OR PROVNPI</t>
+  </si>
+  <si>
+    <t>PID_PDE SNPSHT_DT</t>
+  </si>
+  <si>
+    <t>Merge Variable(s)</t>
+  </si>
+  <si>
+    <t>Information on RVU's and appointment info for provider level encounters</t>
+  </si>
+  <si>
+    <t>Comprehensive Ambulatory Provider Encounter Record</t>
+  </si>
+  <si>
+    <t>provider encounter</t>
+  </si>
+  <si>
+    <t>Standard Inpatient Data Record</t>
+  </si>
+  <si>
+    <t>provider information related to an inpatient stay</t>
+  </si>
+  <si>
+    <t>Inpatient Admission</t>
+  </si>
+  <si>
+    <t>DMIS_PATIENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRICARE Encounter Data; each record is a hospital claim for services provided in the private sector. </t>
+  </si>
+  <si>
+    <t>TRICARE Encounter Data; each record is a non-denied line item claim for services (other than hospital or institutional care for inpatients) provided in the private sector.</t>
+  </si>
+  <si>
+    <t>Provider claim (one cpt per claim)</t>
+  </si>
+  <si>
+    <t>provider encounter (multiple cpt)</t>
+  </si>
+  <si>
+    <t>Multiple Files</t>
+  </si>
+  <si>
+    <t>4 Files each for Army, Non-Army, and Dependents due to STATA size limitations</t>
+  </si>
+  <si>
+    <t>Separate Files for Army, Non-Army and Dependents</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Personnnel Files</t>
+  </si>
+  <si>
+    <t>Separate Files for Army, and other services</t>
+  </si>
+  <si>
+    <t>TEDNO, ADMTEDNO</t>
+  </si>
+  <si>
+    <t>Pharmacy Transactions - not complete before 2011</t>
+  </si>
+  <si>
+    <t>Prescription Dispensed</t>
   </si>
 </sst>
 </file>
@@ -809,6 +921,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1154,11 +1452,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>

</xml_diff>